<commit_message>
change absolute pos fixed
</commit_message>
<xml_diff>
--- a/RevitDynamo/10files/changed_values.xlsx
+++ b/RevitDynamo/10files/changed_values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmsil\Desktop\bsp3\RevitDynamo\10files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565C9448-84AB-4429-9D4E-3E0EBBE2DF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C3E296-363E-4D6C-A52E-FCF32ECD40DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A7A23B64-5B2A-4164-A763-E7FBE671D2B7}"/>
+    <workbookView xWindow="17070" yWindow="3375" windowWidth="19605" windowHeight="15345" xr2:uid="{A7A23B64-5B2A-4164-A763-E7FBE671D2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Wall" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
   <si>
     <t>StairsID</t>
   </si>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B344F34B-228C-4475-BC9D-74856CAA60FC}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +533,7 @@
     <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -585,14 +585,8 @@
       <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -643,12 +637,6 @@
       </c>
       <c r="Q2">
         <v>20350.113000000001</v>
-      </c>
-      <c r="R2">
-        <v>20088</v>
-      </c>
-      <c r="S2">
-        <v>20354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>